<commit_message>
Published state of ETDataset on 8 July 2014.
</commit_message>
<xml_diff>
--- a/analyses/9_agriculture_analysis.xlsx
+++ b/analyses/9_agriculture_analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15400" tabRatio="911" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15960" tabRatio="911" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -7283,9 +7283,7 @@
   </sheetPr>
   <dimension ref="B2:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -7365,7 +7363,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E11" s="296" t="e">
-        <f>D11/SUM($D$11:$D$13)</f>
+        <f>IF(SUM($D$11:$D$13)=0,0,D11/SUM($D$11:$D$13))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7379,7 +7377,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E12" s="296" t="e">
-        <f>D12/SUM($D$11:$D$13)</f>
+        <f>IF(SUM($D$11:$D$13)=0,0,D12/SUM($D$11:$D$13))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7393,7 +7391,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E13" s="296" t="e">
-        <f>D13/SUM($D$11:$D$13)</f>
+        <f>IF(SUM($D$11:$D$13)=0,1,D13/SUM($D$11:$D$13))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -10082,9 +10080,7 @@
   </sheetPr>
   <dimension ref="B2:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>